<commit_message>
Replace sales.xlsx with more data
</commit_message>
<xml_diff>
--- a/data/sales.xlsx
+++ b/data/sales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yijin\Documents\Jin\Princeton\Academics\2024 Fall\COS436\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yubimamiya/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34105B7E-4A82-4D3F-846D-9091B210AF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C05677-FE85-8341-8903-636081F6380B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="8625" windowHeight="10643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="19420" windowHeight="13640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>Date</t>
   </si>
@@ -361,18 +361,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -380,7 +380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45554</v>
       </c>
@@ -388,7 +388,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45555</v>
       </c>
@@ -396,7 +396,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45556</v>
       </c>
@@ -404,7 +404,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45557</v>
       </c>
@@ -412,7 +412,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>45558</v>
       </c>
@@ -420,7 +420,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45559</v>
       </c>
@@ -428,7 +428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>45560</v>
       </c>
@@ -436,7 +436,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>45561</v>
       </c>
@@ -444,7 +444,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>45562</v>
       </c>
@@ -452,7 +452,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>45563</v>
       </c>
@@ -460,7 +460,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>45564</v>
       </c>
@@ -468,13 +468,272 @@
         <v>220</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>45565</v>
       </c>
       <c r="B13">
         <v>210</v>
       </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>45566</v>
+      </c>
+      <c r="B14">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>45567</v>
+      </c>
+      <c r="B15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>45568</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>45569</v>
+      </c>
+      <c r="B17">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>45570</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>45571</v>
+      </c>
+      <c r="B19">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>45572</v>
+      </c>
+      <c r="B20">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>45573</v>
+      </c>
+      <c r="B21">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>45574</v>
+      </c>
+      <c r="B22">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>45575</v>
+      </c>
+      <c r="B23">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>45576</v>
+      </c>
+      <c r="B24">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>45577</v>
+      </c>
+      <c r="B25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>45578</v>
+      </c>
+      <c r="B26">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>45579</v>
+      </c>
+      <c r="B27">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>45580</v>
+      </c>
+      <c r="B28">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>45581</v>
+      </c>
+      <c r="B29">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B30">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>45583</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>45584</v>
+      </c>
+      <c r="B32">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>45585</v>
+      </c>
+      <c r="B33">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>45586</v>
+      </c>
+      <c r="B34">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>45587</v>
+      </c>
+      <c r="B35">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>45588</v>
+      </c>
+      <c r="B36">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update sales.xlsx with correct dates
</commit_message>
<xml_diff>
--- a/data/sales.xlsx
+++ b/data/sales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yubimamiya/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C05677-FE85-8341-8903-636081F6380B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FA29ACF-7BB0-D541-A585-80A88589329C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="19420" windowHeight="13640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,7 +363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>

</xml_diff>